<commit_message>
Added full e2e test of the add book flow. Next i will be implementing this using TestNG
</commit_message>
<xml_diff>
--- a/src/main/java/org/restassured/ExcelTestData.xlsx
+++ b/src/main/java/org/restassured/ExcelTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinorukele/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinorukele/Javaprojects/gitjavaprojects/Rest-Assured-Project/src/main/java/org/restassured/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D32B7B40-2FA0-FE40-A946-234B6208EEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBC2C95-0930-594D-AC18-02F504417246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34160" yWindow="1380" windowWidth="23160" windowHeight="16940" xr2:uid="{85EFEA14-DC77-D34F-AD4E-058EECAABE45}"/>
+    <workbookView xWindow="44260" yWindow="6180" windowWidth="23160" windowHeight="16940" xr2:uid="{85EFEA14-DC77-D34F-AD4E-058EECAABE45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Testcases</t>
   </si>
@@ -63,19 +63,31 @@
   </si>
   <si>
     <t>Kevin O</t>
+  </si>
+  <si>
+    <t>delete-book</t>
+  </si>
+  <si>
+    <t>bc887d1000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC0FF93-FB41-6D41-87C4-9296BA446600}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,6 +472,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>